<commit_message>
Changed total bcq nomination file
</commit_message>
<xml_diff>
--- a/contestable_energy.xlsx
+++ b/contestable_energy.xlsx
@@ -438,7 +438,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>5597.0385765805</v>
+        <v>5799.800999999999</v>
       </c>
     </row>
     <row r="3">
@@ -446,7 +446,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>5427.810091879</v>
+        <v>5649.136500000001</v>
       </c>
     </row>
     <row r="4">
@@ -454,7 +454,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>5378.673491737501</v>
+        <v>5554.8325</v>
       </c>
     </row>
     <row r="5">
@@ -462,7 +462,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>5348.731399226001</v>
+        <v>5481.98</v>
       </c>
     </row>
     <row r="6">
@@ -470,7 +470,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>5372.321170922</v>
+        <v>5456.8815</v>
       </c>
     </row>
     <row r="7">
@@ -478,7 +478,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>5496.759895401</v>
+        <v>5512.395</v>
       </c>
     </row>
     <row r="8">
@@ -486,7 +486,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>6441.069913339</v>
+        <v>5765.477227722772</v>
       </c>
     </row>
     <row r="9">
@@ -494,7 +494,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>7184.668538918501</v>
+        <v>6519.4465</v>
       </c>
     </row>
     <row r="10">
@@ -502,7 +502,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>8465.353500000001</v>
+        <v>7901.5895</v>
       </c>
     </row>
     <row r="11">
@@ -510,7 +510,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>14333.5385</v>
+        <v>13052.0005</v>
       </c>
     </row>
     <row r="12">
@@ -518,7 +518,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>15915.495</v>
+        <v>14886.7985</v>
       </c>
     </row>
     <row r="13">
@@ -526,7 +526,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>15771.6165</v>
+        <v>14810.005</v>
       </c>
     </row>
     <row r="14">
@@ -534,7 +534,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>15824.06</v>
+        <v>14699.3385</v>
       </c>
     </row>
     <row r="15">
@@ -542,7 +542,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>15963.6205</v>
+        <v>15357.636</v>
       </c>
     </row>
     <row r="16">
@@ -550,7 +550,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>16132.936</v>
+        <v>15432.207</v>
       </c>
     </row>
     <row r="17">
@@ -558,7 +558,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>16102.835</v>
+        <v>15338.9075</v>
       </c>
     </row>
     <row r="18">
@@ -566,7 +566,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>16787.6375</v>
+        <v>15792.80217625723</v>
       </c>
     </row>
     <row r="19">
@@ -574,7 +574,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>16403.816</v>
+        <v>15557.50171551809</v>
       </c>
     </row>
     <row r="20">
@@ -582,7 +582,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>16006.496</v>
+        <v>15152.49877462994</v>
       </c>
     </row>
     <row r="21">
@@ -590,7 +590,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>14046.071</v>
+        <v>13812.90902852661</v>
       </c>
     </row>
     <row r="22">
@@ -598,7 +598,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>11183.005</v>
+        <v>12007.84432898735</v>
       </c>
     </row>
     <row r="23">
@@ -606,7 +606,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>9240.505000000001</v>
+        <v>9523.143</v>
       </c>
     </row>
     <row r="24">
@@ -614,7 +614,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>6857.7675</v>
+        <v>6375.7855</v>
       </c>
     </row>
     <row r="25">
@@ -622,7 +622,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>6096.6435</v>
+        <v>5494.996500000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Replaced contestable energy file
</commit_message>
<xml_diff>
--- a/contestable_energy.xlsx
+++ b/contestable_energy.xlsx
@@ -438,7 +438,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>5799.800999999999</v>
+        <v>5597.0385765805</v>
       </c>
     </row>
     <row r="3">
@@ -446,7 +446,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>5649.136500000001</v>
+        <v>5427.810091879</v>
       </c>
     </row>
     <row r="4">
@@ -454,7 +454,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>5554.8325</v>
+        <v>5378.673491737501</v>
       </c>
     </row>
     <row r="5">
@@ -462,7 +462,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>5481.98</v>
+        <v>5348.731399226001</v>
       </c>
     </row>
     <row r="6">
@@ -470,7 +470,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>5456.8815</v>
+        <v>5372.321170922</v>
       </c>
     </row>
     <row r="7">
@@ -478,7 +478,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>5512.395</v>
+        <v>5496.759895401</v>
       </c>
     </row>
     <row r="8">
@@ -486,7 +486,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>5765.477227722772</v>
+        <v>6441.069913339</v>
       </c>
     </row>
     <row r="9">
@@ -494,7 +494,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>6519.4465</v>
+        <v>7184.668538918501</v>
       </c>
     </row>
     <row r="10">
@@ -502,7 +502,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>7901.5895</v>
+        <v>8465.353500000001</v>
       </c>
     </row>
     <row r="11">
@@ -510,7 +510,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>13052.0005</v>
+        <v>14333.5385</v>
       </c>
     </row>
     <row r="12">
@@ -518,7 +518,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>14886.7985</v>
+        <v>15915.495</v>
       </c>
     </row>
     <row r="13">
@@ -526,7 +526,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>14810.005</v>
+        <v>15771.6165</v>
       </c>
     </row>
     <row r="14">
@@ -534,7 +534,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>14699.3385</v>
+        <v>15824.06</v>
       </c>
     </row>
     <row r="15">
@@ -542,7 +542,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>15357.636</v>
+        <v>15963.6205</v>
       </c>
     </row>
     <row r="16">
@@ -550,7 +550,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>15432.207</v>
+        <v>16132.936</v>
       </c>
     </row>
     <row r="17">
@@ -558,7 +558,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>15338.9075</v>
+        <v>16102.835</v>
       </c>
     </row>
     <row r="18">
@@ -566,7 +566,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>15792.80217625723</v>
+        <v>16787.6375</v>
       </c>
     </row>
     <row r="19">
@@ -574,7 +574,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>15557.50171551809</v>
+        <v>16403.816</v>
       </c>
     </row>
     <row r="20">
@@ -582,7 +582,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>15152.49877462994</v>
+        <v>16006.496</v>
       </c>
     </row>
     <row r="21">
@@ -590,7 +590,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>13812.90902852661</v>
+        <v>14046.071</v>
       </c>
     </row>
     <row r="22">
@@ -598,7 +598,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>12007.84432898735</v>
+        <v>11183.005</v>
       </c>
     </row>
     <row r="23">
@@ -606,7 +606,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>9523.143</v>
+        <v>9240.505000000001</v>
       </c>
     </row>
     <row r="24">
@@ -614,7 +614,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>6375.7855</v>
+        <v>6857.7675</v>
       </c>
     </row>
     <row r="25">
@@ -622,7 +622,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>5494.996500000001</v>
+        <v>6096.6435</v>
       </c>
     </row>
   </sheetData>

</xml_diff>